<commit_message>
Updated API Route Plan to be more RESTful
Resources and sub-resources
</commit_message>
<xml_diff>
--- a/01-Planning/ApiRoutePlan.xlsx
+++ b/01-Planning/ApiRoutePlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\comp3000\01-Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF34CF7B-F67E-4695-AEC8-CC11C56F1627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4B83A-1C1F-45AF-91C5-D454187DA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
   <si>
     <t>Method</t>
   </si>
@@ -87,15 +87,9 @@
     <t>Memberships</t>
   </si>
   <si>
-    <t>api/memberships/club/:clubId</t>
-  </si>
-  <si>
     <t>Lists members of a club</t>
   </si>
   <si>
-    <t>api/memberships/user/:userId</t>
-  </si>
-  <si>
     <t>Lists clubs a user is a member of</t>
   </si>
   <si>
@@ -108,15 +102,9 @@
     <t>userId in request body</t>
   </si>
   <si>
-    <t>Elevated permissions needed</t>
-  </si>
-  <si>
     <t>Elevated permissions or self needed</t>
   </si>
   <si>
-    <t>Ends a membership</t>
-  </si>
-  <si>
     <t>api/memberships/club/:clubId/user/:userId</t>
   </si>
   <si>
@@ -147,18 +135,9 @@
     <t>Get invites received for a user</t>
   </si>
   <si>
-    <t>api/invites/:inviteId/accept</t>
-  </si>
-  <si>
-    <t>api/invites/:inviteId/decline</t>
-  </si>
-  <si>
     <t>Updates status</t>
   </si>
   <si>
-    <t>Accept invite, create membership</t>
-  </si>
-  <si>
     <t>api/invites/:inviteId</t>
   </si>
   <si>
@@ -168,9 +147,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>api/invites/user/:userId</t>
-  </si>
-  <si>
     <t>EmergencyContacts</t>
   </si>
   <si>
@@ -189,21 +165,12 @@
     <t>api/emergency-contacts/</t>
   </si>
   <si>
-    <t>api/emergency-contacts/user/:userId</t>
-  </si>
-  <si>
-    <t>Self or admin</t>
-  </si>
-  <si>
     <t>Self</t>
   </si>
   <si>
     <t>api/emergency-contacts/:id</t>
   </si>
   <si>
-    <t>List users emergency contacts</t>
-  </si>
-  <si>
     <t>Update a contact</t>
   </si>
   <si>
@@ -213,9 +180,6 @@
     <t>Create a new contact</t>
   </si>
   <si>
-    <t>api/scores/user/:userId</t>
-  </si>
-  <si>
     <t>api/scores/:id</t>
   </si>
   <si>
@@ -225,27 +189,15 @@
     <t>Update a specific score</t>
   </si>
   <si>
-    <t>List all scores from a user</t>
-  </si>
-  <si>
     <t>Delete a score</t>
   </si>
   <si>
-    <t>api/scores/club/:clubId</t>
-  </si>
-  <si>
-    <t>List all scores from all club members</t>
-  </si>
-  <si>
     <t>Self or elevated</t>
   </si>
   <si>
     <t>api/records-summary/:userId</t>
   </si>
   <si>
-    <t>Get summary</t>
-  </si>
-  <si>
     <t>Update summary</t>
   </si>
   <si>
@@ -264,17 +216,44 @@
     <t>api/clubs/:clubId/memberships</t>
   </si>
   <si>
-    <t>Wrapped "convenience" route</t>
-  </si>
-  <si>
     <t>TODO</t>
+  </si>
+  <si>
+    <t>Accept or decline invite, create membership</t>
+  </si>
+  <si>
+    <t>api/memberships?userId=:userId</t>
+  </si>
+  <si>
+    <t>api/memberships</t>
+  </si>
+  <si>
+    <t>clubId and userId in request body</t>
+  </si>
+  <si>
+    <t>api/invites?userId=:userId</t>
+  </si>
+  <si>
+    <t>api/clubs/:clubId/scores</t>
+  </si>
+  <si>
+    <t>api/memberships/:id</t>
+  </si>
+  <si>
+    <t>Gets a specific membership</t>
+  </si>
+  <si>
+    <t>Whilst membership does have an `id` field, composite of (userId, clubId) where ended_at is null should be preferred.</t>
+  </si>
+  <si>
+    <t>Ends a membership, `ended_at` soft delete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +265,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,15 +303,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,16 +619,16 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -700,10 +690,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,10 +698,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,10 +706,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,16 +718,16 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -755,10 +736,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,10 +747,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,10 +758,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,10 +769,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -802,440 +783,381 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
+      <c r="A26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
         <v>57</v>
       </c>
-      <c r="C40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D55" t="s">
         <v>58</v>
       </c>
-      <c r="D41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" t="s">
-        <v>73</v>
-      </c>
-      <c r="D61" t="s">
-        <v>74</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E48:J48"/>
     <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="A55:D55"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="D26:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
API: Refactor invites route into more RESTful hierarchal URLs
</commit_message>
<xml_diff>
--- a/01-Planning/ApiRoutePlan.xlsx
+++ b/01-Planning/ApiRoutePlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\comp3000\01-Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261C3058-69A3-4A69-BF32-2B25CD8B73B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF884A5-D4ED-41C9-A960-DF629D879CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="19785" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
   <si>
     <t>Method</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Invite a member to a club</t>
+  </si>
+  <si>
+    <t>api/profiles/:userId/invites</t>
   </si>
 </sst>
 </file>
@@ -606,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,92 +722,92 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
+      <c r="A17" t="s">
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,57 +815,51 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,220 +867,220 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
       </c>
       <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>76</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
         <v>37</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
       </c>
       <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D47" t="s">
         <v>54</v>
@@ -1091,105 +1088,119 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="5" t="s">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>55</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>56</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="E50:J50"/>
-    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="A54:D54"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="D28:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>